<commit_message>
Completed 5-66, did indirect only. Now doing 5-67...
</commit_message>
<xml_diff>
--- a/Chapter 5/5-66.xlsx
+++ b/Chapter 5/5-66.xlsx
@@ -1,28 +1,199 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\OneDrive\Desktop\Introduction to Financial Accounting\Chapter 5\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE54CB3D-4A67-466B-861E-BF4B8BBD511D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Statement of Cash Flow" sheetId="1" r:id="rId1"/>
+    <sheet name="Analysis" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+  <si>
+    <t>STATEMENT OF CASH FLOW (in millions of $)</t>
+  </si>
+  <si>
+    <t>Name : Feinstein Company</t>
+  </si>
+  <si>
+    <t>December 31, 2014</t>
+  </si>
+  <si>
+    <t>Particulars</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>CASH Provided (used) By Operations</t>
+  </si>
+  <si>
+    <t>Net Income</t>
+  </si>
+  <si>
+    <t>Adjustments to net income to reconcile</t>
+  </si>
+  <si>
+    <t>with net cash from operations:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Income not affecting cash:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         Depreciation &amp; amortization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Changes in assets &amp; liabilities:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         Increase in Accounts Recievables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         Increase in Inventory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         Increase in Pre-paid Expenses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         Decrease in Accounts Payable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         Decrease in Accrued Taxes Payable</t>
+  </si>
+  <si>
+    <t>Cash Provided By Operations</t>
+  </si>
+  <si>
+    <t>CASH Provided (used) By Investments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Purchase of new plants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Selling of old properties &amp; equipments</t>
+  </si>
+  <si>
+    <t>Cash Used By Investments</t>
+  </si>
+  <si>
+    <t>CASH Provided (used) By Finances</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Proceeds from Long Term Debts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Dividends Paid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    </t>
+  </si>
+  <si>
+    <t>Cash Provided By Finances</t>
+  </si>
+  <si>
+    <t>Net Changes in Cash &amp; Equivalent</t>
+  </si>
+  <si>
+    <t>Cash &amp; Cash Equivalents on 31 Dec 2013</t>
+  </si>
+  <si>
+    <t>Cash &amp; Cash Equivalents on 31 Dec 2014</t>
+  </si>
+  <si>
+    <t>Analysis of Cash Flow Patterns</t>
+  </si>
+  <si>
+    <t>The analysis of cash flow patterns indicates a very interesting thing about</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the nature of the corporation. The management has been so aggressive in </t>
+  </si>
+  <si>
+    <t xml:space="preserve">expanding the business that they purchased a huge consignment of the </t>
+  </si>
+  <si>
+    <t xml:space="preserve">plants without generating sufficient revenue. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The result of these cash flows suggested that the company Is in strongly </t>
+  </si>
+  <si>
+    <t xml:space="preserve">investment stage. So, Mr. Feinstein was certainly right in getting angry </t>
+  </si>
+  <si>
+    <t xml:space="preserve">initially seeing a huge discrepancy in the income and cash flow. However, </t>
+  </si>
+  <si>
+    <t>there is a lot of future investment, in the form of fixed assets, and huge amount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">of potential inventory. Thus, this could well be offset by the initial </t>
+  </si>
+  <si>
+    <t>investment done now.</t>
+  </si>
+  <si>
+    <t>In fact, many companies mantained a negative cash flows for years before</t>
+  </si>
+  <si>
+    <t xml:space="preserve">finally becoming positive. This is, hence, not a big deal. </t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -49,8 +220,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +514,316 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="G5:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N43" sqref="N43"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="7" max="7" width="25.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="7:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="I5" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G7" t="s">
+        <v>1</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H9" s="3"/>
+      <c r="J9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K9" s="4"/>
+    </row>
+    <row r="11" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G11" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K13" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G19" t="s">
+        <v>10</v>
+      </c>
+      <c r="K19">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G22" t="s">
+        <v>13</v>
+      </c>
+      <c r="K22">
+        <v>-21</v>
+      </c>
+    </row>
+    <row r="23" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G23" t="s">
+        <v>14</v>
+      </c>
+      <c r="K23">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="24" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G24" t="s">
+        <v>15</v>
+      </c>
+      <c r="K24">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="25" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G25" t="s">
+        <v>16</v>
+      </c>
+      <c r="K25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G26" t="s">
+        <v>17</v>
+      </c>
+      <c r="K26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G28" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K28" s="5">
+        <f>SUM(K13:K27)</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G30" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G32" t="s">
+        <v>20</v>
+      </c>
+      <c r="K32">
+        <v>-103</v>
+      </c>
+    </row>
+    <row r="33" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G33" t="s">
+        <v>21</v>
+      </c>
+      <c r="K33">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G35" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K35" s="5">
+        <f>SUM(K32:K34)</f>
+        <v>-97</v>
+      </c>
+    </row>
+    <row r="37" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G37" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G39" t="s">
+        <v>24</v>
+      </c>
+      <c r="K39">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G40" t="s">
+        <v>25</v>
+      </c>
+      <c r="K40">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="41" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G41" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="42" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G42" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K42" s="5">
+        <f>SUM(K39:K41)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G44" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K44" s="5">
+        <f>SUM(K28, K35, K42)</f>
+        <v>-18</v>
+      </c>
+    </row>
+    <row r="45" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G45" t="s">
+        <v>29</v>
+      </c>
+      <c r="K45">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G47" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H47" s="5"/>
+      <c r="I47" s="5"/>
+      <c r="J47" s="5"/>
+      <c r="K47" s="5">
+        <f>SUM(K44:K46)</f>
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="J9:K9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE877D76-CF43-4967-B952-627A1FE7DEC0}">
+  <dimension ref="F6:F21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="6" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F6" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>